<commit_message>
For LI to be saved with the new 3 fields in the tmf also fixed some missing parameters in function BPRO, still needed the logtra file changes
</commit_message>
<xml_diff>
--- a/Transactions - Stream/IPS-LI-TMF (transactions saved).xlsx
+++ b/Transactions - Stream/IPS-LI-TMF (transactions saved).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\105864\Documents\Millennium\Transactions - Stream\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C5E696B-E265-4964-911B-282E76250ECE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E5A9E7-A3F9-4B25-A5A4-A192929E404D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9F2AF06A-391B-40AD-9C34-9E017E47FE0C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="122">
   <si>
     <t>TRABUF(TITYP).EQ.IVAL</t>
   </si>
@@ -305,6 +305,99 @@
   </si>
   <si>
     <t>0xD5 (OIFIN.FOR)</t>
+  </si>
+  <si>
+    <t>IVAL</t>
+  </si>
+  <si>
+    <t>Batch Validation (7 tickets max)</t>
+  </si>
+  <si>
+    <t>[4  7]</t>
+  </si>
+  <si>
+    <t>[2  3]</t>
+  </si>
+  <si>
+    <t>[1]</t>
+  </si>
+  <si>
+    <t>3 segmentos em uso</t>
+  </si>
+  <si>
+    <t>2 segmentos em uso</t>
+  </si>
+  <si>
+    <t>LOGBUF posições em uso</t>
+  </si>
+  <si>
+    <t>LOGBUF(9),LOGBUF(32),LOGBUF(48)</t>
+  </si>
+  <si>
+    <t>LOGBUF(9),LOGBUF(31),LOGBUF(32)</t>
+  </si>
+  <si>
+    <t>LOGBUF(9),LOGBUF(17),LOGBUF(18)</t>
+  </si>
+  <si>
+    <t>range (min - max)</t>
+  </si>
+  <si>
+    <t>Para o melhor dos casos só está 4 tickets em uso ou sejá teria o 3º segmento livre mas sendo necessario os 9 bytes seriam sempre usados 3 bytes no 3º segmento para esse efeito contempla-se o pior dos casos estar a ser usados 7 tickets estão só LOGBUF(48) disponívels</t>
+  </si>
+  <si>
+    <t>4 tickets LOGBUF(33) até LOGBUF(47) livres</t>
+  </si>
+  <si>
+    <t>5 tickets LOGBUF(38) até LOGBUF(47) livres</t>
+  </si>
+  <si>
+    <t>6 tickets LOGBUF(43) até LOGBUF(47) livres</t>
+  </si>
+  <si>
+    <t>7 tickets estão todas as posições do LOGBUF em uso</t>
+  </si>
+  <si>
+    <t>Sendo o caso de 2 tickets em uso está livre o LOGBUF(22) até LOGBUF(31), no caso de 3 tickets é LOGBUF(27) até LOGBUF(31) tendo então as 5 posições 27,28,29,30,31 livres mais a posição 32 então escolheu-se o 32 que é por regra usado e o campo 31 para ficar logo colado ao 32</t>
+  </si>
+  <si>
+    <t>Estado só um ticket é necessario os 2 segmentos pois é necessario ainda 6 bytes para o serial number do Olimpo estando disponível todo o 2 segmento escolhendo logo os primeiros 2 campos 17,18</t>
+  </si>
+  <si>
+    <t>ILOT</t>
+  </si>
+  <si>
+    <t>Alteração Estado Maço</t>
+  </si>
+  <si>
+    <t>LOGBUF(14),LOGBUF(15),LOGBUF(17),LOGBUF(18),  LOGBUF(19),LOGBUF(20)</t>
+  </si>
+  <si>
+    <t>SIZE 1 to SIZE 2 of segments needed</t>
+  </si>
+  <si>
+    <t>TRABUF(TIBCH).GE.4</t>
+  </si>
+  <si>
+    <t>TRABUF(TIBCH).GE.1.AND.TRABUF(TIBCH).LT.4</t>
+  </si>
+  <si>
+    <t>ICAR</t>
+  </si>
+  <si>
+    <t>Activação Caixa de Jogo LI</t>
+  </si>
+  <si>
+    <t>IQTA</t>
+  </si>
+  <si>
+    <t>LOGBUF(10),LOGBUF(11),LOGBUF(12),LOGBUF(13),  LOGBUF(14),LOGBUF(15)</t>
+  </si>
+  <si>
+    <t>SIZE 1 and keeps being Size 1 segment needed</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -366,25 +459,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -399,38 +480,68 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -460,7 +571,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>2476266</xdr:colOff>
+      <xdr:colOff>2476267</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>20317</xdr:rowOff>
     </xdr:to>
@@ -487,6 +598,182 @@
         <a:xfrm>
           <a:off x="608135" y="223959"/>
           <a:ext cx="5654965" cy="895396"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>179614</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2440504</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>11589</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagem 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10CB781C-1BE0-4447-B0E3-7B1145B3C6E5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="7184571"/>
+          <a:ext cx="5613689" cy="4864350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>5443</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2449122</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>27401</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagem 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{656FF104-8013-4698-BB5E-3C16F60A05AA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="615043" y="12034157"/>
+          <a:ext cx="5613689" cy="3622861"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>306903</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>11590</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagem 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{576B4412-72F3-4C87-852D-022DED21D1CA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11027229" y="7004957"/>
+          <a:ext cx="5613689" cy="4858000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>124114</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>8415</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagem 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3AB49F5-CF57-4946-9C6E-5DE641569475}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18037629" y="7004957"/>
+          <a:ext cx="5613689" cy="4861175"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -795,629 +1082,968 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F9357B7-F398-410C-BF75-8CC0928D0E2B}">
-  <dimension ref="A1:O31"/>
+  <dimension ref="A1:Q110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD18"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="23" customWidth="1"/>
     <col min="5" max="5" width="19.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="46.26953125" customWidth="1"/>
     <col min="7" max="7" width="50.54296875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.453125" customWidth="1"/>
     <col min="11" max="11" width="13.08984375" customWidth="1"/>
+    <col min="17" max="17" width="15.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="K1" s="5"/>
+      <c r="K1" s="16"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" s="9">
+      <c r="A2" s="5">
         <v>8</v>
       </c>
-      <c r="H2" s="9">
+      <c r="H2" s="5">
         <v>13</v>
       </c>
-      <c r="I2" s="9">
+      <c r="I2" s="5">
         <v>2</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="K2" s="5"/>
+      <c r="K2" s="16"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="H3" s="9">
+      <c r="H3" s="5">
         <v>13</v>
       </c>
-      <c r="I3" s="9">
+      <c r="I3" s="5">
         <v>3</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="K3" s="5"/>
+      <c r="K3" s="16"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="H4" s="9">
+      <c r="H4" s="5">
         <v>13</v>
       </c>
-      <c r="I4" s="9">
+      <c r="I4" s="5">
         <v>6</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="K4" s="5"/>
+      <c r="K4" s="16"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="H5" s="9">
+      <c r="H5" s="5">
         <v>13</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I5" s="5">
         <v>7</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="K5" s="5"/>
+      <c r="K5" s="16"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="H6" s="9">
+      <c r="H6" s="5">
         <v>13</v>
       </c>
-      <c r="I6" s="9">
+      <c r="I6" s="5">
         <v>8</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="K6" s="5"/>
+      <c r="K6" s="16"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="H7" s="9">
+      <c r="H7" s="5">
         <v>13</v>
       </c>
-      <c r="I7" s="9">
+      <c r="I7" s="5">
         <v>12</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J7" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="K7" s="5"/>
+      <c r="K7" s="16"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="H8" s="9">
+      <c r="H8" s="5">
         <v>13</v>
       </c>
-      <c r="I8" s="9">
+      <c r="I8" s="5">
         <v>13</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="J8" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="K8" s="5"/>
+      <c r="K8" s="16"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="H9" s="9">
+      <c r="H9" s="5">
         <v>13</v>
       </c>
-      <c r="I9" s="9">
+      <c r="I9" s="5">
         <v>14</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="J9" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="K9" s="5"/>
+      <c r="K9" s="16"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
       <c r="E11" s="1" t="s">
         <v>62</v>
       </c>
       <c r="F11" s="1"/>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="20" t="s">
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="20" t="s">
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="F13" s="14"/>
-      <c r="G13" s="8" t="s">
+      <c r="F13" s="8"/>
+      <c r="G13" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="H13" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="21"/>
+      <c r="O13" s="21"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="20" t="s">
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="H14" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="21"/>
+      <c r="O14" s="21"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="20" t="s">
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="F15" s="14"/>
-      <c r="G15" s="8" t="s">
+      <c r="F15" s="8"/>
+      <c r="G15" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H15" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="21"/>
+      <c r="N15" s="21"/>
+      <c r="O15" s="21"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="20" t="s">
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="F16" s="14"/>
-      <c r="G16" s="8" t="s">
+      <c r="F16" s="8"/>
+      <c r="G16" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="21"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="21"/>
+      <c r="M16" s="21"/>
+      <c r="N16" s="21"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="19" t="s">
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="F17" s="15"/>
-      <c r="G17" s="8" t="s">
+      <c r="F17" s="9"/>
+      <c r="G17" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="H17" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="21"/>
+      <c r="L17" s="21"/>
+      <c r="M17" s="21"/>
+      <c r="N17" s="21"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="17" t="s">
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="G18" s="8" t="s">
+      <c r="G18" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="H18" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="21"/>
+      <c r="M18" s="21"/>
+      <c r="N18" s="21"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="19" t="s">
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="F19" s="15"/>
-      <c r="G19" s="8" t="s">
+      <c r="F19" s="9"/>
+      <c r="G19" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="H19" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
+      <c r="M19" s="21"/>
+      <c r="N19" s="21"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="19" t="s">
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="F20" s="15"/>
-      <c r="G20" s="8" t="s">
+      <c r="F20" s="9"/>
+      <c r="G20" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="H20" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="21"/>
+      <c r="L20" s="21"/>
+      <c r="M20" s="21"/>
+      <c r="N20" s="21"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="20" t="s">
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="F21" s="14"/>
-      <c r="G21" s="8" t="s">
+      <c r="F21" s="8"/>
+      <c r="G21" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="H21" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="21"/>
+      <c r="L21" s="21"/>
+      <c r="M21" s="21"/>
+      <c r="N21" s="21"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="20" t="s">
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="G22" s="8" t="s">
+      <c r="G22" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="H22" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="21"/>
+      <c r="K22" s="21"/>
+      <c r="L22" s="21"/>
+      <c r="M22" s="21"/>
+      <c r="N22" s="21"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="18" t="s">
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="F23" s="16"/>
-      <c r="G23" s="8" t="s">
+      <c r="F23" s="10"/>
+      <c r="G23" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="H23" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="21"/>
+      <c r="K23" s="21"/>
+      <c r="L23" s="21"/>
+      <c r="M23" s="21"/>
+      <c r="N23" s="21"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="19" t="s">
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="F24" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G24" s="8" t="s">
+      <c r="G24" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="H24" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="21"/>
+      <c r="L24" s="21"/>
+      <c r="M24" s="21"/>
+      <c r="N24" s="21"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="19" t="s">
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="F25" s="15"/>
-      <c r="G25" s="8" t="s">
+      <c r="F25" s="9"/>
+      <c r="G25" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="H25" s="3" t="s">
+      <c r="H25" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
+      <c r="L25" s="21"/>
+      <c r="M25" s="21"/>
+      <c r="N25" s="21"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="17" t="s">
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="F26" s="15"/>
-      <c r="G26" s="8" t="s">
+      <c r="F26" s="9"/>
+      <c r="G26" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="H26" s="7" t="s">
+      <c r="H26" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="7"/>
-      <c r="M26" s="7"/>
-      <c r="N26" s="7"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A27" s="19" t="s">
+      <c r="A27" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="19" t="s">
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="F27" s="11" t="s">
+      <c r="F27" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="G27" s="8" t="s">
+      <c r="G27" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="H27" s="3" t="s">
+      <c r="H27" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
-      <c r="N27" s="3"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="21"/>
+      <c r="L27" s="21"/>
+      <c r="M27" s="21"/>
+      <c r="N27" s="21"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B28" s="21" t="s">
+      <c r="B28" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="9" t="s">
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="F28" s="9"/>
+      <c r="F28" s="5"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B29" s="21" t="s">
+      <c r="B29" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="22" t="s">
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="F29" s="22"/>
+      <c r="F29" s="19"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B36" t="s">
+        <v>91</v>
+      </c>
+      <c r="C36" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D36" s="23"/>
+      <c r="E36" s="23"/>
+      <c r="F36" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>114</v>
+      </c>
+      <c r="B37" t="s">
+        <v>93</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" ht="31" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="B38" t="s">
+        <v>94</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B39" t="s">
+        <v>95</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+      <c r="F39" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>102</v>
+      </c>
+      <c r="G40" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>93</v>
+      </c>
+      <c r="G41" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="G43" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q43" s="27" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A44" s="25"/>
+      <c r="G44" s="26"/>
+      <c r="Q44" s="27"/>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A45" s="25"/>
+      <c r="G45" s="26"/>
+      <c r="Q45" s="27"/>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A46" s="25"/>
+      <c r="G46" s="26"/>
+      <c r="Q46" s="27"/>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A47" s="25"/>
+      <c r="G47" s="26"/>
+      <c r="Q47" s="27"/>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A48" s="25"/>
+      <c r="Q48" s="27"/>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A49" s="25"/>
+      <c r="Q49" s="27"/>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A50" s="25"/>
+      <c r="Q50" s="27"/>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A51" s="25"/>
+      <c r="Q51" s="27"/>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A52" s="25"/>
+      <c r="Q52" s="27"/>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A53" s="25"/>
+      <c r="Q53" s="27"/>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A54" s="25"/>
+      <c r="Q54" s="27"/>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A55" s="25"/>
+      <c r="Q55" s="27"/>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A56" s="25"/>
+      <c r="Q56" s="27"/>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A57" s="25"/>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A58" s="25"/>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A59" s="25"/>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A60" s="25"/>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A62" s="25" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A63" s="25"/>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A64" s="25"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A66" s="26" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A67" s="26"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A68" s="26"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A70" s="26" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A71" s="26"/>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A72" s="26"/>
+    </row>
+    <row r="74" spans="1:1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="26" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A75" s="26"/>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A76" s="26"/>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A77" s="26"/>
+    </row>
+    <row r="90" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B90" t="s">
+        <v>110</v>
+      </c>
+      <c r="C90" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="D90" s="26"/>
+      <c r="E90" s="26"/>
+      <c r="F90" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="91" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F91" s="26" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="92" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F92" s="26"/>
+    </row>
+    <row r="93" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F93" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="96" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B96" t="s">
+        <v>116</v>
+      </c>
+      <c r="C96" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="D96" s="26"/>
+      <c r="E96" s="26"/>
+      <c r="F96" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="97" spans="2:6" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F97" s="28" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="98" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F98" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="101" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B101" t="s">
+        <v>118</v>
+      </c>
+      <c r="C101" s="26"/>
+      <c r="D101" s="26"/>
+      <c r="E101" s="26"/>
+      <c r="F101" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="102" spans="2:6" ht="37" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F102" s="28" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="103" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F103" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="109" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E109">
+        <v>20</v>
+      </c>
+      <c r="F109" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="110" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E110">
+        <v>15</v>
+      </c>
+      <c r="F110">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="46">
+  <mergeCells count="61">
+    <mergeCell ref="C96:E96"/>
+    <mergeCell ref="C101:E101"/>
+    <mergeCell ref="G43:G47"/>
+    <mergeCell ref="Q43:Q56"/>
+    <mergeCell ref="C90:E90"/>
+    <mergeCell ref="F91:F92"/>
+    <mergeCell ref="A62:A64"/>
+    <mergeCell ref="A66:A68"/>
+    <mergeCell ref="A70:A72"/>
+    <mergeCell ref="A74:A77"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="A43:A60"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="H12:M12"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="H11:M11"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="H13:O13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="H14:O14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="H15:O15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="H16:N16"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="H22:N22"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J5:K5"/>
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="J7:K7"/>
     <mergeCell ref="J8:K8"/>
@@ -1429,41 +2055,11 @@
     <mergeCell ref="H24:N24"/>
     <mergeCell ref="H25:N25"/>
     <mergeCell ref="H27:N27"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J5:K5"/>
     <mergeCell ref="H17:N17"/>
     <mergeCell ref="H18:N18"/>
     <mergeCell ref="H19:N19"/>
     <mergeCell ref="H20:N20"/>
     <mergeCell ref="H21:N21"/>
-    <mergeCell ref="H22:N22"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="H14:O14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="H15:O15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="H16:N16"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="H12:M12"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="H11:M11"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="H13:O13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>